<commit_message>
1. added mcmc 2. added hadoop type checker 3. updated configuration settings
</commit_message>
<xml_diff>
--- a/resource/hadoop_params.xlsx
+++ b/resource/hadoop_params.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\aws\sysopt\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\FSE18\code\sysopt\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9086,7 +9086,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -9483,11 +9483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A973" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B996" sqref="B996"/>
+    <sheetView tabSelected="1" topLeftCell="A916" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A956" sqref="A956"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>